<commit_message>
Criando Conexao ao Banco de Dados
</commit_message>
<xml_diff>
--- a/AppEstacionamento/Dados/Dados.xlsx
+++ b/AppEstacionamento/Dados/Dados.xlsx
@@ -14,12 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <x:si>
-    <x:t>Gizelli</x:t>
-  </x:si>
-  <x:si>
-    <x:t>877.872.112-74</x:t>
+    <x:t>henderson</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -370,32 +367,15 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:C3"/>
+  <x:dimension ref="A1:D6"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="2" spans="1:3">
-      <x:c r="A2" s="0" t="n">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="B2" s="0" t="s">
+    <x:row r="2" spans="1:4">
+      <x:c r="A2" s="0" t="s">
         <x:v>0</x:v>
-      </x:c>
-      <x:c r="C2" s="0" t="s">
-        <x:v>1</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:3">
-      <x:c r="A3" s="0" t="n">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="B3" s="0" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="C3" s="0" t="s">
-        <x:v>1</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>